<commit_message>
Hoàn thành chức năng thêm danh muc
</commit_message>
<xml_diff>
--- a/document/PhieuChamDiem.xlsx
+++ b/document/PhieuChamDiem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="6780" activeTab="1"/>
+    <workbookView windowWidth="19635" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Decriptions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="134">
   <si>
     <t>Tên nhóm:</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>HIỆN DANH XỬ LÍ VI PHẠM</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
   <si>
     <t>LIÊN KẾT ID ĐỂ NGƯỜI SAU THỰC HIỆN CHỨC NĂNG TIẾP THEO , HIỆN BAO GỒM CÁC TAB SỐ LIỆU THỐNG KÊ</t>
@@ -1148,6 +1151,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1169,7 +1175,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2415,8 +2420,8 @@
   <sheetPr/>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -2451,7 +2456,7 @@
       <c r="B2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3" t="s">
         <v>82</v>
       </c>
@@ -2464,7 +2469,7 @@
       <c r="B3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="3" t="s">
         <v>84</v>
       </c>
@@ -2477,7 +2482,7 @@
       <c r="B4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="3" t="s">
         <v>86</v>
       </c>
@@ -2490,7 +2495,7 @@
       <c r="B5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="3" t="s">
         <v>88</v>
       </c>
@@ -2503,7 +2508,7 @@
       <c r="B6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="3" t="s">
         <v>90</v>
       </c>
@@ -2516,7 +2521,7 @@
       <c r="B7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="3" t="s">
         <v>92</v>
       </c>
@@ -2529,7 +2534,7 @@
       <c r="B8" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
@@ -2540,7 +2545,7 @@
       <c r="B9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
@@ -2551,7 +2556,7 @@
       <c r="B10" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="3" t="s">
         <v>96</v>
       </c>
@@ -2564,7 +2569,7 @@
       <c r="B11" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
@@ -2575,7 +2580,7 @@
       <c r="B12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
@@ -2586,7 +2591,7 @@
       <c r="B13" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="3" t="s">
         <v>100</v>
       </c>
@@ -2599,7 +2604,7 @@
       <c r="B14" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="3" t="s">
         <v>102</v>
       </c>
@@ -2612,7 +2617,7 @@
       <c r="B15" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="3" t="s">
         <v>104</v>
       </c>
@@ -2625,7 +2630,7 @@
       <c r="B16" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="3" t="s">
         <v>106</v>
       </c>
@@ -2638,7 +2643,7 @@
       <c r="B17" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
@@ -2649,7 +2654,7 @@
       <c r="B18" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="3" t="s">
         <v>109</v>
       </c>
@@ -2662,7 +2667,7 @@
       <c r="B19" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
@@ -2673,7 +2678,7 @@
       <c r="B20" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="3" t="s">
         <v>109</v>
       </c>
@@ -2686,7 +2691,7 @@
       <c r="B21" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="3" t="s">
         <v>109</v>
       </c>
@@ -2699,7 +2704,7 @@
       <c r="B22" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="3" t="s">
         <v>109</v>
       </c>
@@ -2712,9 +2717,11 @@
       <c r="B23" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D23" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -2723,11 +2730,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C24" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D24" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -2736,11 +2745,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D25" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E25" s="3"/>
     </row>
@@ -2749,9 +2760,11 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
@@ -2760,9 +2773,9 @@
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="C27" s="4"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
@@ -2771,9 +2784,9 @@
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
@@ -2782,9 +2795,9 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="C29" s="4"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
@@ -2793,47 +2806,47 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="C30" s="4"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
+      <c r="A31" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="A32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="11">
+      <c r="A34" s="12">
         <v>1</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="11" t="s">
-        <v>128</v>
+      <c r="D34" s="12" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2841,11 +2854,11 @@
         <v>2</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2853,10 +2866,10 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix lai hien thi bai viet
</commit_message>
<xml_diff>
--- a/document/PhieuChamDiem.xlsx
+++ b/document/PhieuChamDiem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="6780" activeTab="1"/>
+    <workbookView windowWidth="19635" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Decriptions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="134">
   <si>
     <t>Tên nhóm:</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>HIỆN DANH XỬ LÍ VI PHẠM</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
   <si>
     <t>LIÊN KẾT ID ĐỂ NGƯỜI SAU THỰC HIỆN CHỨC NĂNG TIẾP THEO , HIỆN BAO GỒM CÁC TAB SỐ LIỆU THỐNG KÊ</t>
@@ -1148,6 +1151,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1169,7 +1175,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2415,8 +2420,8 @@
   <sheetPr/>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -2451,7 +2456,7 @@
       <c r="B2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3" t="s">
         <v>82</v>
       </c>
@@ -2464,7 +2469,7 @@
       <c r="B3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="3" t="s">
         <v>84</v>
       </c>
@@ -2477,7 +2482,7 @@
       <c r="B4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="3" t="s">
         <v>86</v>
       </c>
@@ -2490,7 +2495,7 @@
       <c r="B5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="3" t="s">
         <v>88</v>
       </c>
@@ -2503,7 +2508,7 @@
       <c r="B6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="3" t="s">
         <v>90</v>
       </c>
@@ -2516,7 +2521,7 @@
       <c r="B7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="3" t="s">
         <v>92</v>
       </c>
@@ -2529,7 +2534,7 @@
       <c r="B8" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
@@ -2540,7 +2545,7 @@
       <c r="B9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
@@ -2551,7 +2556,7 @@
       <c r="B10" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="3" t="s">
         <v>96</v>
       </c>
@@ -2564,7 +2569,7 @@
       <c r="B11" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
@@ -2575,7 +2580,7 @@
       <c r="B12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
@@ -2586,7 +2591,7 @@
       <c r="B13" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="3" t="s">
         <v>100</v>
       </c>
@@ -2599,7 +2604,7 @@
       <c r="B14" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="3" t="s">
         <v>102</v>
       </c>
@@ -2612,7 +2617,7 @@
       <c r="B15" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="3" t="s">
         <v>104</v>
       </c>
@@ -2625,7 +2630,7 @@
       <c r="B16" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="3" t="s">
         <v>106</v>
       </c>
@@ -2638,7 +2643,7 @@
       <c r="B17" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
@@ -2649,7 +2654,7 @@
       <c r="B18" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="3" t="s">
         <v>109</v>
       </c>
@@ -2662,7 +2667,7 @@
       <c r="B19" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
@@ -2673,7 +2678,7 @@
       <c r="B20" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="3" t="s">
         <v>109</v>
       </c>
@@ -2686,7 +2691,7 @@
       <c r="B21" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="3" t="s">
         <v>109</v>
       </c>
@@ -2699,7 +2704,7 @@
       <c r="B22" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="3" t="s">
         <v>109</v>
       </c>
@@ -2712,9 +2717,11 @@
       <c r="B23" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D23" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -2723,11 +2730,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C24" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D24" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -2736,11 +2745,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D25" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E25" s="3"/>
     </row>
@@ -2749,9 +2760,11 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
@@ -2760,9 +2773,9 @@
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="C27" s="4"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
@@ -2771,9 +2784,9 @@
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
@@ -2782,9 +2795,9 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="C29" s="4"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
@@ -2793,47 +2806,47 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="C30" s="4"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
+      <c r="A31" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="A32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="11">
+      <c r="A34" s="12">
         <v>1</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="11" t="s">
-        <v>128</v>
+      <c r="D34" s="12" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2841,11 +2854,11 @@
         <v>2</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2853,10 +2866,10 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>